<commit_message>
concept voor eerste werkgroep addendum gp2019
</commit_message>
<xml_diff>
--- a/output/GWC_gp2019.xlsx
+++ b/output/GWC_gp2019.xlsx
@@ -7,40 +7,11 @@
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="GWC" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
-  <si>
-    <t>Criterium</t>
-  </si>
-  <si>
-    <t>max</t>
-  </si>
-  <si>
-    <t>mean</t>
-  </si>
-  <si>
-    <t>min</t>
-  </si>
-  <si>
-    <t>Won 58 dB(A) Lden</t>
-  </si>
-  <si>
-    <t>EGH 48 dB(A) Lden</t>
-  </si>
-  <si>
-    <t>Won 48 dB(A) Lnight</t>
-  </si>
-  <si>
-    <t>SV 40 dB(A) Lnight</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -395,86 +366,107 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Criterium</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>mean</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>max</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>min</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>meteomarge</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Won 58 dB(A) Lden</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>10200</v>
       </c>
       <c r="C2" t="n">
-        <v>9400</v>
+        <v>10800</v>
       </c>
       <c r="D2" t="n">
-        <v>9100</v>
+        <v>9700</v>
       </c>
       <c r="E2" t="n">
-        <v>8700</v>
+        <v>11300</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>EGH 48 dB(A) Lden</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>98800</v>
       </c>
       <c r="C3" t="n">
-        <v>149200</v>
+        <v>103000</v>
       </c>
       <c r="D3" t="n">
-        <v>137500</v>
+        <v>94800</v>
       </c>
       <c r="E3" t="n">
-        <v>124600</v>
+        <v>112000</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Won 48 dB(A) Lnight</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>7300</v>
       </c>
       <c r="C4" t="n">
-        <v>7400</v>
+        <v>8400</v>
       </c>
       <c r="D4" t="n">
-        <v>6200</v>
+        <v>6000</v>
       </c>
       <c r="E4" t="n">
-        <v>2700</v>
+        <v>9000</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>SV 40 dB(A) Lnight</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>20600</v>
       </c>
       <c r="C5" t="n">
-        <v>24300</v>
+        <v>22300</v>
       </c>
       <c r="D5" t="n">
-        <v>22400</v>
+        <v>19400</v>
       </c>
       <c r="E5" t="n">
-        <v>21000</v>
+        <v>24200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>